<commit_message>
force npc fix bell & cora
</commit_message>
<xml_diff>
--- a/gu_in/Map.edf/neutralB.xlsx
+++ b/gu_in/Map.edf/neutralB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\emay.dev\Parser_1.0.2\Database\gu_in\Map.edf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8CF655-424F-4492-94D6-A1818F913FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C21C9E4-027A-44CB-9882-A467664AA3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32570,8 +32570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="F148" sqref="F148"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32717,7 +32717,7 @@
         <v>-5323</v>
       </c>
       <c r="D6" s="1">
-        <v>575</v>
+        <v>200575</v>
       </c>
       <c r="E6" s="1">
         <v>6039</v>
@@ -33133,7 +33133,7 @@
         <v>-5338</v>
       </c>
       <c r="D22" s="1">
-        <v>574</v>
+        <v>200574</v>
       </c>
       <c r="E22" s="1">
         <v>6113</v>

</xml_diff>